<commit_message>
Add final analysis, update code.
</commit_message>
<xml_diff>
--- a/spec_props/spcor_assembly.xlsx
+++ b/spec_props/spcor_assembly.xlsx
@@ -9,13 +9,14 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="192">
   <si>
     <t>Abbreviation</t>
   </si>
@@ -138,6 +139,9 @@
   </si>
   <si>
     <t>http://datadryad.org/resource/doi:10.5061/dryad.846nj</t>
+  </si>
+  <si>
+    <t>Computed from reference genome</t>
   </si>
   <si>
     <t>bmor</t>
@@ -723,29 +727,23 @@
   </sheetPr>
   <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="6387" ySplit="0" topLeftCell="T1" activePane="topRight" state="split"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="V22" activeCellId="0" sqref="V22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.015306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="19.3571428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="26.6734693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.0663265306122"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="16.9897959183673"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="10.8061224489796"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="21.3928571428571"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="13.9591836734694"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.90816326530612"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="13.2857142857143"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="13.734693877551"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="76.4336734693878"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="1" width="19.1326530612245"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="22.219387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="1" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.9948979591837"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="8.8265306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.5051020408163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.1632653061224"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="8.8265306122449"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="19.8367346938776"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="17.1632653061224"/>
+    <col collapsed="false" hidden="false" max="14" min="10" style="1" width="8.8265306122449"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="14.1632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="1" width="8.8265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -853,7 +851,6 @@
       <c r="P2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Q2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
@@ -966,7 +963,6 @@
       <c r="P4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Q4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
@@ -1020,7 +1016,6 @@
       <c r="P5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Q5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
@@ -1035,16 +1030,22 @@
       <c r="D6" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="0"/>
-      <c r="G6" s="5" t="e">
+      <c r="E6" s="5" t="n">
+        <v>463349471</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>420897271</v>
+      </c>
+      <c r="G6" s="5" t="n">
         <f aca="false">F6/E6</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5" t="e">
+        <v>0.908379737850181</v>
+      </c>
+      <c r="H6" s="5" t="n">
+        <v>410805174</v>
+      </c>
+      <c r="I6" s="5" t="n">
         <f aca="false">H6/F6</f>
-        <v>#DIV/0!</v>
+        <v>0.976022422345428</v>
       </c>
       <c r="J6" s="1" t="n">
         <v>21</v>
@@ -1063,35 +1064,42 @@
       <c r="N6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="O6" s="0"/>
+      <c r="O6" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="P6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Q6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5" t="e">
+        <v>44</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>502962945</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>502962945</v>
+      </c>
+      <c r="G7" s="5" t="n">
         <f aca="false">F7/E7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5" t="e">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1" t="n">
+        <v>377177827</v>
+      </c>
+      <c r="I7" s="5" t="n">
         <f aca="false">H7/F7</f>
-        <v>#DIV/0!</v>
+        <v>0.749911759404065</v>
       </c>
       <c r="J7" s="1" t="n">
         <v>27</v>
@@ -1104,40 +1112,47 @@
         <v>513.45</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="N7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="O7" s="0"/>
+      <c r="O7" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="P7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Q7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" s="0"/>
-      <c r="F8" s="0"/>
-      <c r="G8" s="5" t="e">
+        <v>48</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>273790497</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>221851317</v>
+      </c>
+      <c r="G8" s="5" t="n">
         <f aca="false">F8/E8</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5" t="e">
+        <v>0.81029589934964</v>
+      </c>
+      <c r="H8" s="5" t="n">
+        <v>218680715</v>
+      </c>
+      <c r="I8" s="5" t="n">
         <f aca="false">H8/F8</f>
-        <v>#DIV/0!</v>
+        <v>0.985708437331476</v>
       </c>
       <c r="J8" s="1" t="n">
         <v>20</v>
@@ -1150,29 +1165,30 @@
         <v>293.4</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="N8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="O8" s="0"/>
+      <c r="O8" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="P8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Q8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E9" s="5" t="n">
         <v>1412448247</v>
@@ -1203,7 +1219,7 @@
         <v>1713.945</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="N9" s="2" t="s">
         <v>21</v>
@@ -1214,20 +1230,19 @@
       <c r="P9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Q9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E10" s="1" t="n">
         <v>1061800384</v>
@@ -1258,10 +1273,10 @@
         <v>1431.14</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>22</v>
@@ -1269,20 +1284,19 @@
       <c r="P10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Q10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E11" s="5" t="n">
         <v>2474912402</v>
@@ -1313,7 +1327,7 @@
         <v>3117.864</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="N11" s="2" t="s">
         <v>21</v>
@@ -1324,20 +1338,19 @@
       <c r="P11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Q11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E12" s="5" t="n">
         <v>265011681</v>
@@ -1367,7 +1380,7 @@
         <v>264.06</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N12" s="2" t="s">
         <v>21</v>
@@ -1378,20 +1391,19 @@
       <c r="P12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Q12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E13" s="5" t="n">
         <v>2410960148</v>
@@ -1421,7 +1433,7 @@
         <v>2748.18</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="N13" s="2" t="s">
         <v>21</v>
@@ -1432,20 +1444,19 @@
       <c r="P13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Q13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E14" s="1" t="n">
         <v>314353944</v>
@@ -1475,7 +1486,7 @@
         <v>469.44</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="N14" s="2" t="s">
         <v>21</v>
@@ -1484,22 +1495,21 @@
         <v>22</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q14" s="0"/>
+        <v>76</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E15" s="5" t="n">
         <v>1046915324</v>
@@ -1529,10 +1539,10 @@
         <v>1222.5</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="O15" s="1" t="s">
         <v>22</v>
@@ -1540,20 +1550,19 @@
       <c r="P15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Q15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E16" s="1" t="n">
         <v>945861706</v>
@@ -1583,7 +1592,7 @@
         <v>1369.2</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="N16" s="2" t="s">
         <v>21</v>
@@ -1594,20 +1603,19 @@
       <c r="P16" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Q16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E17" s="1" t="n">
         <v>3101788170</v>
@@ -1637,7 +1645,7 @@
         <v>3423</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="N17" s="2" t="s">
         <v>21</v>
@@ -1648,20 +1656,19 @@
       <c r="P17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Q17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E18" s="1" t="n">
         <v>2948380710</v>
@@ -1691,7 +1698,7 @@
         <v>3452.34</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="N18" s="2" t="s">
         <v>21</v>
@@ -1703,21 +1710,21 @@
         <v>23</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E19" s="1" t="n">
         <v>869801494</v>
@@ -1747,7 +1754,7 @@
         <v>1056.24</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="N19" s="2" t="s">
         <v>21</v>
@@ -1758,20 +1765,19 @@
       <c r="P19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Q19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E20" s="1" t="n">
         <v>2730855475</v>
@@ -1801,7 +1807,7 @@
         <v>3002.46</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="N20" s="2" t="s">
         <v>21</v>
@@ -1813,21 +1819,21 @@
         <v>23</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E21" s="5" t="n">
         <v>250270657</v>
@@ -1858,7 +1864,7 @@
         <v>249.39</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="N21" s="2" t="s">
         <v>21</v>
@@ -1869,20 +1875,19 @@
       <c r="P21" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Q21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E22" s="1" t="n">
         <v>3097370727</v>
@@ -1913,7 +1918,7 @@
         <v>3290.97</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="N22" s="2" t="s">
         <v>21</v>
@@ -1924,20 +1929,19 @@
       <c r="P22" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Q22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E23" s="1" t="n">
         <v>2808509378</v>
@@ -1967,7 +1971,7 @@
         <v>2748.18</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="N23" s="2" t="s">
         <v>21</v>
@@ -1979,21 +1983,21 @@
         <v>23</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E24" s="5" t="n">
         <v>2670405961</v>
@@ -2023,10 +2027,10 @@
         <v>3569.7</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="O24" s="1" t="s">
         <v>22</v>
@@ -2034,20 +2038,19 @@
       <c r="P24" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Q24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E25" s="1" t="n">
         <v>2619037772</v>
@@ -2077,7 +2080,7 @@
         <v>3227.4</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="N25" s="2" t="s">
         <v>21</v>
@@ -2088,31 +2091,36 @@
       <c r="P25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Q25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5" t="e">
+        <v>127</v>
+      </c>
+      <c r="E26" s="1" t="n">
+        <v>301388396</v>
+      </c>
+      <c r="F26" s="1" t="n">
+        <v>288587601</v>
+      </c>
+      <c r="G26" s="5" t="n">
         <f aca="false">F26/E26</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5" t="e">
+        <v>0.957527246669444</v>
+      </c>
+      <c r="H26" s="1" t="n">
+        <v>283837116</v>
+      </c>
+      <c r="I26" s="5" t="n">
         <f aca="false">H26/F26</f>
-        <v>#DIV/0!</v>
+        <v>0.983538845800932</v>
       </c>
       <c r="J26" s="1" t="n">
         <v>9</v>
@@ -2125,42 +2133,50 @@
         <v>469.44</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="O26" s="0"/>
+        <v>58</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="P26" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5" t="e">
+        <v>96</v>
+      </c>
+      <c r="E27" s="1" t="n">
+        <v>134835427</v>
+      </c>
+      <c r="F27" s="1" t="n">
+        <v>124881110</v>
+      </c>
+      <c r="G27" s="5" t="n">
         <f aca="false">F27/E27</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5" t="e">
+        <v>0.926174320640524</v>
+      </c>
+      <c r="H27" s="1" t="n">
+        <v>123232065</v>
+      </c>
+      <c r="I27" s="5" t="n">
         <f aca="false">H27/F27</f>
-        <v>#DIV/0!</v>
+        <v>0.986795080537</v>
       </c>
       <c r="J27" s="1" t="n">
         <v>8</v>
@@ -2173,40 +2189,47 @@
         <v>215.16</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="N27" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="O27" s="0"/>
+      <c r="O27" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="P27" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q27" s="0"/>
+        <v>76</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E28" s="0"/>
-      <c r="F28" s="0"/>
-      <c r="G28" s="5" t="e">
+        <v>135</v>
+      </c>
+      <c r="E28" s="1" t="n">
+        <v>761407154</v>
+      </c>
+      <c r="F28" s="1" t="n">
+        <v>749228103</v>
+      </c>
+      <c r="G28" s="5" t="n">
         <f aca="false">F28/E28</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5" t="e">
+        <v>0.984004548767347</v>
+      </c>
+      <c r="H28" s="5" t="n">
+        <v>737837083</v>
+      </c>
+      <c r="I28" s="5" t="n">
         <f aca="false">H28/F28</f>
-        <v>#DIV/0!</v>
+        <v>0.984796325772633</v>
       </c>
       <c r="J28" s="1" t="n">
         <v>13</v>
@@ -2219,40 +2242,47 @@
         <v>880.2</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="N28" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="O28" s="0"/>
+      <c r="O28" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="P28" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q28" s="0"/>
+        <v>76</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="E29" s="0"/>
-      <c r="F29" s="0"/>
-      <c r="G29" s="5" t="e">
+        <v>139</v>
+      </c>
+      <c r="E29" s="1" t="n">
+        <v>218265040</v>
+      </c>
+      <c r="F29" s="1" t="n">
+        <v>218265040</v>
+      </c>
+      <c r="G29" s="5" t="n">
         <f aca="false">F29/E29</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5" t="e">
+        <v>1</v>
+      </c>
+      <c r="H29" s="5" t="n">
+        <v>215929111</v>
+      </c>
+      <c r="I29" s="5" t="n">
         <f aca="false">H29/F29</f>
-        <v>#DIV/0!</v>
+        <v>0.989297740948344</v>
       </c>
       <c r="J29" s="1" t="n">
         <v>8</v>
@@ -2265,42 +2295,50 @@
         <v>303.18</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="N29" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="O29" s="0"/>
+      <c r="O29" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="P29" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="E30" s="0"/>
-      <c r="F30" s="0"/>
-      <c r="G30" s="5" t="e">
+        <v>144</v>
+      </c>
+      <c r="E30" s="1" t="n">
+        <v>434136308</v>
+      </c>
+      <c r="F30" s="1" t="n">
+        <v>394507750</v>
+      </c>
+      <c r="G30" s="5" t="n">
         <f aca="false">F30/E30</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5" t="e">
+        <v>0.908718627606701</v>
+      </c>
+      <c r="H30" s="5" t="n">
+        <v>387934746</v>
+      </c>
+      <c r="I30" s="5" t="n">
         <f aca="false">H30/F30</f>
-        <v>#DIV/0!</v>
+        <v>0.983338720215256</v>
       </c>
       <c r="J30" s="1" t="n">
         <v>19</v>
@@ -2313,40 +2351,47 @@
         <v>479.22</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="N30" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="O30" s="0"/>
+      <c r="O30" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="P30" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q30" s="0"/>
+        <v>76</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E31" s="0"/>
-      <c r="F31" s="0"/>
-      <c r="G31" s="5" t="e">
+        <v>135</v>
+      </c>
+      <c r="E31" s="1" t="n">
+        <v>405737677</v>
+      </c>
+      <c r="F31" s="1" t="n">
+        <v>401300885</v>
+      </c>
+      <c r="G31" s="5" t="n">
         <f aca="false">F31/E31</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5" t="e">
+        <v>0.989064875530403</v>
+      </c>
+      <c r="H31" s="5" t="n">
+        <v>396684774</v>
+      </c>
+      <c r="I31" s="5" t="n">
         <f aca="false">H31/F31</f>
-        <v>#DIV/0!</v>
+        <v>0.988497132270217</v>
       </c>
       <c r="J31" s="1" t="n">
         <v>9</v>
@@ -2359,40 +2404,47 @@
         <v>518.34</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="N31" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="O31" s="0"/>
+        <v>58</v>
+      </c>
+      <c r="O31" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="P31" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q31" s="0"/>
+        <v>76</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="E32" s="0"/>
-      <c r="F32" s="0"/>
-      <c r="G32" s="5" t="e">
+        <v>152</v>
+      </c>
+      <c r="E32" s="1" t="n">
+        <v>374471254</v>
+      </c>
+      <c r="F32" s="1" t="n">
+        <v>373245531</v>
+      </c>
+      <c r="G32" s="5" t="n">
         <f aca="false">F32/E32</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H32" s="5"/>
-      <c r="I32" s="5" t="e">
+        <v>0.996726790142348</v>
+      </c>
+      <c r="H32" s="5" t="n">
+        <v>373128865</v>
+      </c>
+      <c r="I32" s="5" t="n">
         <f aca="false">H32/F32</f>
-        <v>#DIV/0!</v>
+        <v>0.999687428273588</v>
       </c>
       <c r="J32" s="1" t="n">
         <v>12</v>
@@ -2405,42 +2457,50 @@
         <v>449.88</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="N32" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="O32" s="0"/>
+      <c r="O32" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="P32" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5" t="e">
+        <v>157</v>
+      </c>
+      <c r="E33" s="5" t="n">
+        <v>197284272</v>
+      </c>
+      <c r="F33" s="5" t="n">
+        <v>191859031</v>
+      </c>
+      <c r="G33" s="5" t="n">
         <f aca="false">F33/E33</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H33" s="5"/>
-      <c r="I33" s="5" t="e">
+        <v>0.972500387663949</v>
+      </c>
+      <c r="H33" s="5" t="n">
+        <v>188626844</v>
+      </c>
+      <c r="I33" s="5" t="n">
         <f aca="false">H33/F33</f>
-        <v>#DIV/0!</v>
+        <v>0.983153323650425</v>
       </c>
       <c r="J33" s="1" t="n">
         <v>7</v>
@@ -2453,40 +2513,47 @@
         <v>880.2</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="N33" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="O33" s="0"/>
+      <c r="O33" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="P33" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q33" s="0"/>
+        <v>76</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E34" s="0"/>
-      <c r="F34" s="0"/>
-      <c r="G34" s="5" t="e">
+        <v>96</v>
+      </c>
+      <c r="E34" s="1" t="n">
+        <v>355247431</v>
+      </c>
+      <c r="F34" s="1" t="n">
+        <v>355247431</v>
+      </c>
+      <c r="G34" s="5" t="n">
         <f aca="false">F34/E34</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H34" s="5"/>
-      <c r="I34" s="5" t="e">
+        <v>1</v>
+      </c>
+      <c r="H34" s="5" t="n">
+        <v>321373230</v>
+      </c>
+      <c r="I34" s="5" t="n">
         <f aca="false">H34/F34</f>
-        <v>#DIV/0!</v>
+        <v>0.904646176033853</v>
       </c>
       <c r="J34" s="1" t="n">
         <v>11</v>
@@ -2499,31 +2566,33 @@
         <v>440.1</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="N34" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="O34" s="0"/>
+      <c r="O34" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="P34" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="Q34" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E35" s="5" t="n">
         <v>271923306</v>
@@ -2553,7 +2622,7 @@
         <v>352.08</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="N35" s="2" t="s">
         <v>21</v>
@@ -2562,22 +2631,21 @@
         <v>22</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q35" s="0"/>
+        <v>76</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E36" s="1" t="n">
         <v>738540932</v>
@@ -2607,7 +2675,7 @@
         <v>733.5</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="N36" s="2" t="s">
         <v>21</v>
@@ -2616,22 +2684,21 @@
         <v>22</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q36" s="0"/>
+        <v>76</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E37" s="1" t="n">
         <v>2065703473</v>
@@ -2661,7 +2728,7 @@
         <v>2669.94</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="N37" s="2" t="s">
         <v>21</v>
@@ -2670,22 +2737,21 @@
         <v>22</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q37" s="0"/>
+        <v>76</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E38" s="5" t="n">
         <v>119146348</v>
@@ -2715,7 +2781,7 @@
         <v>156.48</v>
       </c>
       <c r="M38" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="N38" s="2" t="s">
         <v>21</v>
@@ -2724,22 +2790,21 @@
         <v>22</v>
       </c>
       <c r="P38" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q38" s="0"/>
+        <v>76</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E39" s="1" t="n">
         <v>973340353</v>
@@ -2769,7 +2834,7 @@
         <v>1105.14</v>
       </c>
       <c r="M39" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="N39" s="2" t="s">
         <v>21</v>
@@ -2778,22 +2843,21 @@
         <v>22</v>
       </c>
       <c r="P39" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q39" s="0"/>
+        <v>76</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E40" s="1" t="n">
         <v>1118326800</v>
@@ -2824,7 +2888,7 @@
         <v>1275.74666666667</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="N40" s="1" t="s">
         <v>21</v>
@@ -2836,21 +2900,21 @@
         <v>23</v>
       </c>
       <c r="Q40" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E41" s="1" t="n">
         <v>470182763</v>
@@ -2880,7 +2944,7 @@
         <v>606.36</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="N41" s="1" t="s">
         <v>21</v>
@@ -2892,7 +2956,7 @@
         <v>23</v>
       </c>
       <c r="Q41" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -2904,4 +2968,41 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <tabColor rgb="00FFFFFF"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A41" activeCellId="0" sqref="A41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.9948979591837"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.5051020408163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.1632653061224"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.8367346938776"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="8.8265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.7295918367347"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2"/>
+      <c r="F1" s="4"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>